<commit_message>
Fixed GAINS issues. Remove GAINS-EU to keep only GAINS-IAM.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-trucks.xlsx
+++ b/premise/data/additional_inventories/lci-trucks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD8125D-D361-8048-8B59-8100EDC25A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67950329-7060-9541-841A-87D3A9BAC0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="760" windowWidth="24180" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38140" yWindow="160" windowWidth="24180" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2084,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I5092"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1846" workbookViewId="0">
-      <selection activeCell="A1883" sqref="A1883"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2578" sqref="B2578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17275,7 +17275,7 @@
         <v>197</v>
       </c>
       <c r="B967">
-        <v>0.9285714285714286</v>
+        <v>-0.92857142857142905</v>
       </c>
       <c r="C967" t="s">
         <v>425</v>
@@ -18063,7 +18063,7 @@
         <v>197</v>
       </c>
       <c r="B1019">
-        <v>0.9285714285714286</v>
+        <v>-0.92857142857142905</v>
       </c>
       <c r="C1019" t="s">
         <v>425</v>
@@ -19951,7 +19951,7 @@
         <v>197</v>
       </c>
       <c r="B1126">
-        <v>0.9285714285714286</v>
+        <v>-0.92857142857142905</v>
       </c>
       <c r="C1126" t="s">
         <v>425</v>
@@ -22579,7 +22579,7 @@
         <v>197</v>
       </c>
       <c r="B1270">
-        <v>0.9285714285714286</v>
+        <v>-0.92857142857142905</v>
       </c>
       <c r="C1270" t="s">
         <v>425</v>
@@ -23627,7 +23627,7 @@
         <v>197</v>
       </c>
       <c r="B1335">
-        <v>0.9285714285714286</v>
+        <v>-0.92857142857142905</v>
       </c>
       <c r="C1335" t="s">
         <v>425</v>
@@ -25575,7 +25575,7 @@
         <v>197</v>
       </c>
       <c r="B1445">
-        <v>0.9285714285714286</v>
+        <v>-0.92857142857142905</v>
       </c>
       <c r="C1445" t="s">
         <v>425</v>
@@ -36911,7 +36911,7 @@
         <v>197</v>
       </c>
       <c r="B2100">
-        <v>1.142857142857143</v>
+        <v>-1.1428571428571399</v>
       </c>
       <c r="C2100" t="s">
         <v>425</v>
@@ -37699,7 +37699,7 @@
         <v>197</v>
       </c>
       <c r="B2152">
-        <v>1.142857142857143</v>
+        <v>-1.1428571428571399</v>
       </c>
       <c r="C2152" t="s">
         <v>425</v>
@@ -39587,7 +39587,7 @@
         <v>197</v>
       </c>
       <c r="B2259">
-        <v>1.142857142857143</v>
+        <v>-1.1428571428571399</v>
       </c>
       <c r="C2259" t="s">
         <v>425</v>
@@ -42215,7 +42215,7 @@
         <v>197</v>
       </c>
       <c r="B2403">
-        <v>1.142857142857143</v>
+        <v>-1.1428571428571399</v>
       </c>
       <c r="C2403" t="s">
         <v>425</v>
@@ -43263,7 +43263,7 @@
         <v>197</v>
       </c>
       <c r="B2468">
-        <v>1.142857142857143</v>
+        <v>-1.1428571428571399</v>
       </c>
       <c r="C2468" t="s">
         <v>425</v>
@@ -45211,7 +45211,7 @@
         <v>197</v>
       </c>
       <c r="B2578">
-        <v>1.142857142857143</v>
+        <v>-1.1428571428571399</v>
       </c>
       <c r="C2578" t="s">
         <v>425</v>
@@ -45939,7 +45939,7 @@
         <v>235</v>
       </c>
       <c r="B2627">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C2627" t="s">
         <v>425</v>
@@ -46727,7 +46727,7 @@
         <v>235</v>
       </c>
       <c r="B2679">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C2679" t="s">
         <v>425</v>
@@ -47221,7 +47221,7 @@
         <v>235</v>
       </c>
       <c r="B2710">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C2710" t="s">
         <v>425</v>
@@ -47675,7 +47675,7 @@
         <v>235</v>
       </c>
       <c r="B2739">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C2739" t="s">
         <v>425</v>
@@ -48129,7 +48129,7 @@
         <v>235</v>
       </c>
       <c r="B2768">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C2768" t="s">
         <v>425</v>
@@ -50077,7 +50077,7 @@
         <v>235</v>
       </c>
       <c r="B2878">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C2878" t="s">
         <v>425</v>
@@ -50805,7 +50805,7 @@
         <v>235</v>
       </c>
       <c r="B2927">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C2927" t="s">
         <v>425</v>
@@ -51593,7 +51593,7 @@
         <v>235</v>
       </c>
       <c r="B2979">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C2979" t="s">
         <v>425</v>
@@ -53481,7 +53481,7 @@
         <v>235</v>
       </c>
       <c r="B3086">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C3086" t="s">
         <v>425</v>
@@ -56109,7 +56109,7 @@
         <v>235</v>
       </c>
       <c r="B3230">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C3230" t="s">
         <v>425</v>
@@ -57157,7 +57157,7 @@
         <v>235</v>
       </c>
       <c r="B3295">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C3295" t="s">
         <v>425</v>
@@ -59105,7 +59105,7 @@
         <v>235</v>
       </c>
       <c r="B3405">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C3405" t="s">
         <v>425</v>

</xml_diff>